<commit_message>
Images, boutons utilisables ecrit, etc
</commit_message>
<xml_diff>
--- a/Classeur1.xlsx
+++ b/Classeur1.xlsx
@@ -1180,7 +1180,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -1207,7 +1207,10 @@
         <v>20.0</v>
       </c>
       <c r="H1" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
+      </c>
+      <c r="I1" t="n">
+        <v>4.0</v>
       </c>
     </row>
     <row r="2">
@@ -1233,6 +1236,9 @@
       <c r="H2" t="n">
         <v>2.0</v>
       </c>
+      <c r="I2" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
@@ -1257,6 +1263,9 @@
       <c r="H3" t="n">
         <v>2.0</v>
       </c>
+      <c r="I3" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
@@ -1281,6 +1290,9 @@
       <c r="H4" t="n">
         <v>2.0</v>
       </c>
+      <c r="I4" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
@@ -1305,6 +1317,9 @@
       <c r="H5" t="n">
         <v>2.0</v>
       </c>
+      <c r="I5" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
@@ -1329,6 +1344,9 @@
       <c r="H6" t="n">
         <v>2.0</v>
       </c>
+      <c r="I6" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
@@ -1353,6 +1371,9 @@
       <c r="H7" t="n">
         <v>1.0</v>
       </c>
+      <c r="I7" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
@@ -1377,6 +1398,9 @@
       <c r="H8" t="n">
         <v>2.0</v>
       </c>
+      <c r="I8" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
@@ -1401,6 +1425,9 @@
       <c r="H9" t="n">
         <v>2.0</v>
       </c>
+      <c r="I9" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
@@ -1425,6 +1452,9 @@
       <c r="H10" t="n">
         <v>2.0</v>
       </c>
+      <c r="I10" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
@@ -1449,6 +1479,9 @@
       <c r="H11" t="n">
         <v>2.0</v>
       </c>
+      <c r="I11" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
@@ -1473,6 +1506,9 @@
       <c r="H12" t="n">
         <v>2.0</v>
       </c>
+      <c r="I12" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
@@ -1497,6 +1533,9 @@
       <c r="H13" t="n">
         <v>2.0</v>
       </c>
+      <c r="I13" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
@@ -1521,6 +1560,9 @@
       <c r="H14" t="n">
         <v>2.0</v>
       </c>
+      <c r="I14" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
@@ -1545,6 +1587,9 @@
       <c r="H15" t="n">
         <v>2.0</v>
       </c>
+      <c r="I15" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
@@ -1569,6 +1614,9 @@
       <c r="H16" t="n">
         <v>2.0</v>
       </c>
+      <c r="I16" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
@@ -1593,6 +1641,9 @@
       <c r="H17" t="n">
         <v>2.0</v>
       </c>
+      <c r="I17" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
@@ -1617,6 +1668,9 @@
       <c r="H18" t="n">
         <v>2.0</v>
       </c>
+      <c r="I18" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
@@ -1641,6 +1695,9 @@
       <c r="H19" t="n">
         <v>2.0</v>
       </c>
+      <c r="I19" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
@@ -1665,6 +1722,9 @@
       <c r="H20" t="n">
         <v>2.0</v>
       </c>
+      <c r="I20" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
@@ -1689,6 +1749,9 @@
       <c r="H21" t="n">
         <v>2.0</v>
       </c>
+      <c r="I21" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
@@ -1713,6 +1776,9 @@
       <c r="H22" t="n">
         <v>2.0</v>
       </c>
+      <c r="I22" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
@@ -1737,6 +1803,9 @@
       <c r="H23" t="n">
         <v>2.0</v>
       </c>
+      <c r="I23" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
@@ -1761,6 +1830,9 @@
       <c r="H24" t="n">
         <v>2.0</v>
       </c>
+      <c r="I24" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
@@ -1785,6 +1857,9 @@
       <c r="H25" t="n">
         <v>2.0</v>
       </c>
+      <c r="I25" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
@@ -1809,6 +1884,9 @@
       <c r="H26" t="n">
         <v>2.0</v>
       </c>
+      <c r="I26" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
@@ -1831,6 +1909,9 @@
         <v>5.0</v>
       </c>
       <c r="H27" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="I27" t="n">
         <v>2.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
L'ecriture des pouvoirs fonctionnelles
</commit_message>
<xml_diff>
--- a/Classeur1.xlsx
+++ b/Classeur1.xlsx
@@ -12,39 +12,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="27">
   <si>
     <t>4444</t>
   </si>
   <si>
-    <t>Alex</t>
+    <t>bernat</t>
   </si>
   <si>
     <t>rocher</t>
   </si>
   <si>
+    <t>true</t>
+  </si>
+  <si>
     <t>false</t>
-  </si>
-  <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>amos</t>
-  </si>
-  <si>
-    <t>anna</t>
-  </si>
-  <si>
-    <t>annette</t>
-  </si>
-  <si>
-    <t>arthur</t>
-  </si>
-  <si>
-    <t>king</t>
-  </si>
-  <si>
-    <t>bernat</t>
   </si>
   <si>
     <t>bob</t>
@@ -1029,164 +1011,12 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>9006</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="24" name="Picture 1" descr="Picture"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="true"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId24"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="2143125" cy="2143125"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>9006</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="25" name="Picture 1" descr="Picture"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="true"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId25"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="2143125" cy="2143125"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>9006</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="26" name="Picture 1" descr="Picture"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="true"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId26"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="2143125" cy="2143125"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>9006</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="27" name="Picture 1" descr="Picture"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="true"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId27"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="2143125" cy="2143125"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N27"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -1210,28 +1040,28 @@
         <v>1.0</v>
       </c>
       <c r="G1" t="n">
-        <v>20.0</v>
+        <v>15.0</v>
       </c>
       <c r="H1" t="n">
-        <v>9.0</v>
+        <v>6.0</v>
       </c>
       <c r="I1" t="s">
         <v>3</v>
       </c>
       <c r="J1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K1" t="s">
         <v>4</v>
       </c>
       <c r="L1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2">
@@ -1245,32 +1075,32 @@
         <v>0.0</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E2"/>
       <c r="F2" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="G2" t="n">
-        <v>5.0</v>
+        <v>31.0</v>
       </c>
       <c r="H2" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="I2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J2" t="s">
         <v>4</v>
       </c>
       <c r="K2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L2" t="s">
         <v>4</v>
       </c>
       <c r="M2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N2" t="s">
         <v>4</v>
@@ -1281,7 +1111,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" t="n">
         <v>0.0</v>
@@ -1294,28 +1124,28 @@
         <v>1.0</v>
       </c>
       <c r="G3" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="H3" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="I3" t="s">
         <v>4</v>
       </c>
       <c r="J3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
@@ -1323,7 +1153,7 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" t="n">
         <v>0.0</v>
@@ -1342,22 +1172,22 @@
         <v>2.0</v>
       </c>
       <c r="I4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
@@ -1365,13 +1195,13 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E5"/>
       <c r="F5" t="n">
@@ -1384,22 +1214,22 @@
         <v>2.0</v>
       </c>
       <c r="I5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
@@ -1426,22 +1256,22 @@
         <v>2.0</v>
       </c>
       <c r="I6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">
@@ -1455,35 +1285,35 @@
         <v>0.0</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E7"/>
       <c r="F7" t="n">
         <v>1.0</v>
       </c>
       <c r="G7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H7" t="n">
         <v>2.0</v>
       </c>
-      <c r="H7" t="n">
-        <v>1.0</v>
-      </c>
       <c r="I7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8">
@@ -1491,7 +1321,7 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" t="n">
         <v>0.0</v>
@@ -1504,28 +1334,28 @@
         <v>1.0</v>
       </c>
       <c r="G8" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="H8" t="n">
         <v>2.0</v>
       </c>
       <c r="I8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9">
@@ -1533,7 +1363,7 @@
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" t="n">
         <v>0.0</v>
@@ -1552,22 +1382,22 @@
         <v>2.0</v>
       </c>
       <c r="I9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10">
@@ -1575,7 +1405,7 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" t="n">
         <v>0.0</v>
@@ -1588,28 +1418,28 @@
         <v>1.0</v>
       </c>
       <c r="G10" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="H10" t="n">
         <v>2.0</v>
       </c>
       <c r="I10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11">
@@ -1617,7 +1447,7 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" t="n">
         <v>0.0</v>
@@ -1630,28 +1460,28 @@
         <v>1.0</v>
       </c>
       <c r="G11" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="H11" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="I11" t="s">
         <v>4</v>
       </c>
       <c r="J11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12">
@@ -1659,7 +1489,7 @@
         <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C12" t="n">
         <v>0.0</v>
@@ -1672,28 +1502,28 @@
         <v>1.0</v>
       </c>
       <c r="G12" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="H12" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="I12" t="s">
         <v>4</v>
       </c>
       <c r="J12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13">
@@ -1701,7 +1531,7 @@
         <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C13" t="n">
         <v>0.0</v>
@@ -1720,22 +1550,22 @@
         <v>2.0</v>
       </c>
       <c r="I13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14">
@@ -1743,7 +1573,7 @@
         <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C14" t="n">
         <v>0.0</v>
@@ -1762,22 +1592,22 @@
         <v>2.0</v>
       </c>
       <c r="I14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15">
@@ -1785,7 +1615,7 @@
         <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C15" t="n">
         <v>0.0</v>
@@ -1798,28 +1628,28 @@
         <v>1.0</v>
       </c>
       <c r="G15" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="H15" t="n">
         <v>2.0</v>
       </c>
       <c r="I15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16">
@@ -1827,7 +1657,7 @@
         <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C16" t="n">
         <v>0.0</v>
@@ -1846,22 +1676,22 @@
         <v>2.0</v>
       </c>
       <c r="I16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17">
@@ -1869,7 +1699,7 @@
         <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C17" t="n">
         <v>0.0</v>
@@ -1888,22 +1718,22 @@
         <v>2.0</v>
       </c>
       <c r="I17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18">
@@ -1911,7 +1741,7 @@
         <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C18" t="n">
         <v>0.0</v>
@@ -1930,22 +1760,22 @@
         <v>2.0</v>
       </c>
       <c r="I18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19">
@@ -1953,7 +1783,7 @@
         <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C19" t="n">
         <v>0.0</v>
@@ -1972,22 +1802,22 @@
         <v>2.0</v>
       </c>
       <c r="I19" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J19" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K19" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L19" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M19" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N19" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20">
@@ -1995,7 +1825,7 @@
         <v>0</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C20" t="n">
         <v>0.0</v>
@@ -2008,28 +1838,28 @@
         <v>1.0</v>
       </c>
       <c r="G20" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="H20" t="n">
         <v>2.0</v>
       </c>
       <c r="I20" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J20" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K20" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L20" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M20" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N20" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21">
@@ -2037,7 +1867,7 @@
         <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C21" t="n">
         <v>0.0</v>
@@ -2050,28 +1880,28 @@
         <v>1.0</v>
       </c>
       <c r="G21" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="H21" t="n">
         <v>2.0</v>
       </c>
       <c r="I21" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J21" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K21" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L21" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M21" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N21" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22">
@@ -2079,7 +1909,7 @@
         <v>0</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C22" t="n">
         <v>0.0</v>
@@ -2098,22 +1928,22 @@
         <v>2.0</v>
       </c>
       <c r="I22" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J22" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K22" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L22" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M22" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N22" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23">
@@ -2121,7 +1951,7 @@
         <v>0</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C23" t="n">
         <v>0.0</v>
@@ -2134,196 +1964,28 @@
         <v>1.0</v>
       </c>
       <c r="G23" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="H23" t="n">
         <v>2.0</v>
       </c>
       <c r="I23" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J23" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K23" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L23" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M23" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N23" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D24" t="s">
-        <v>2</v>
-      </c>
-      <c r="E24"/>
-      <c r="F24" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="G24" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="H24" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="I24" t="s">
-        <v>4</v>
-      </c>
-      <c r="J24" t="s">
-        <v>4</v>
-      </c>
-      <c r="K24" t="s">
-        <v>4</v>
-      </c>
-      <c r="L24" t="s">
-        <v>4</v>
-      </c>
-      <c r="M24" t="s">
-        <v>4</v>
-      </c>
-      <c r="N24" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s">
-        <v>0</v>
-      </c>
-      <c r="B25" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D25" t="s">
-        <v>2</v>
-      </c>
-      <c r="E25"/>
-      <c r="F25" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="G25" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="H25" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="I25" t="s">
-        <v>4</v>
-      </c>
-      <c r="J25" t="s">
-        <v>4</v>
-      </c>
-      <c r="K25" t="s">
-        <v>4</v>
-      </c>
-      <c r="L25" t="s">
-        <v>4</v>
-      </c>
-      <c r="M25" t="s">
-        <v>4</v>
-      </c>
-      <c r="N25" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26" t="s">
-        <v>31</v>
-      </c>
-      <c r="C26" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D26" t="s">
-        <v>2</v>
-      </c>
-      <c r="E26"/>
-      <c r="F26" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="G26" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="H26" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="I26" t="s">
-        <v>4</v>
-      </c>
-      <c r="J26" t="s">
-        <v>4</v>
-      </c>
-      <c r="K26" t="s">
-        <v>4</v>
-      </c>
-      <c r="L26" t="s">
-        <v>4</v>
-      </c>
-      <c r="M26" t="s">
-        <v>4</v>
-      </c>
-      <c r="N26" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="s">
-        <v>0</v>
-      </c>
-      <c r="B27" t="s">
-        <v>32</v>
-      </c>
-      <c r="C27" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D27" t="s">
-        <v>2</v>
-      </c>
-      <c r="E27"/>
-      <c r="F27" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="G27" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="H27" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="I27" t="s">
-        <v>4</v>
-      </c>
-      <c r="J27" t="s">
-        <v>4</v>
-      </c>
-      <c r="K27" t="s">
-        <v>4</v>
-      </c>
-      <c r="L27" t="s">
-        <v>4</v>
-      </c>
-      <c r="M27" t="s">
-        <v>4</v>
-      </c>
-      <c r="N27" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
quelques problemes avec frameNomRole
</commit_message>
<xml_diff>
--- a/Classeur1.xlsx
+++ b/Classeur1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="27">
   <si>
     <t>4444</t>
   </si>
@@ -21,9 +21,6 @@
   </si>
   <si>
     <t>rocher</t>
-  </si>
-  <si>
-    <t>C:\Users\user\Documents\Projet-informatique-ClassCraft\default.png</t>
   </si>
   <si>
     <t>false</t>
@@ -159,9 +156,7 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
+      <c r="E1"/>
       <c r="F1" t="n">
         <v>1.0</v>
       </c>
@@ -172,22 +167,22 @@
         <v>6.0</v>
       </c>
       <c r="I1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2">
@@ -195,13 +190,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
       </c>
       <c r="E2"/>
       <c r="F2" t="n">
@@ -214,22 +209,22 @@
         <v>4.0</v>
       </c>
       <c r="I2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
@@ -237,7 +232,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" t="n">
         <v>0.0</v>
@@ -256,22 +251,22 @@
         <v>3.0</v>
       </c>
       <c r="I3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
@@ -279,7 +274,7 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="n">
         <v>0.0</v>
@@ -298,22 +293,22 @@
         <v>2.0</v>
       </c>
       <c r="I4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
@@ -321,7 +316,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" t="n">
         <v>0.0</v>
@@ -340,22 +335,22 @@
         <v>2.0</v>
       </c>
       <c r="I5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
@@ -363,7 +358,7 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" t="n">
         <v>0.0</v>
@@ -382,22 +377,22 @@
         <v>2.0</v>
       </c>
       <c r="I6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
@@ -405,7 +400,7 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" t="n">
         <v>0.0</v>
@@ -424,22 +419,22 @@
         <v>2.0</v>
       </c>
       <c r="I7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8">
@@ -447,7 +442,7 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" t="n">
         <v>0.0</v>
@@ -466,22 +461,22 @@
         <v>2.0</v>
       </c>
       <c r="I8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9">
@@ -489,7 +484,7 @@
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" t="n">
         <v>0.0</v>
@@ -508,22 +503,22 @@
         <v>2.0</v>
       </c>
       <c r="I9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10">
@@ -531,7 +526,7 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" t="n">
         <v>0.0</v>
@@ -550,22 +545,22 @@
         <v>2.0</v>
       </c>
       <c r="I10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11">
@@ -573,7 +568,7 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" t="n">
         <v>0.0</v>
@@ -592,22 +587,22 @@
         <v>3.0</v>
       </c>
       <c r="I11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12">
@@ -615,7 +610,7 @@
         <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" t="n">
         <v>0.0</v>
@@ -634,22 +629,22 @@
         <v>3.0</v>
       </c>
       <c r="I12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13">
@@ -657,7 +652,7 @@
         <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" t="n">
         <v>0.0</v>
@@ -676,22 +671,22 @@
         <v>2.0</v>
       </c>
       <c r="I13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14">
@@ -699,7 +694,7 @@
         <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" t="n">
         <v>0.0</v>
@@ -718,22 +713,22 @@
         <v>2.0</v>
       </c>
       <c r="I14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15">
@@ -741,7 +736,7 @@
         <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" t="n">
         <v>0.0</v>
@@ -760,22 +755,22 @@
         <v>2.0</v>
       </c>
       <c r="I15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16">
@@ -783,7 +778,7 @@
         <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" t="n">
         <v>0.0</v>
@@ -802,22 +797,22 @@
         <v>2.0</v>
       </c>
       <c r="I16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17">
@@ -825,7 +820,7 @@
         <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" t="n">
         <v>0.0</v>
@@ -844,22 +839,22 @@
         <v>2.0</v>
       </c>
       <c r="I17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18">
@@ -867,7 +862,7 @@
         <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C18" t="n">
         <v>0.0</v>
@@ -886,22 +881,22 @@
         <v>2.0</v>
       </c>
       <c r="I18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19">
@@ -909,7 +904,7 @@
         <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" t="n">
         <v>0.0</v>
@@ -928,22 +923,22 @@
         <v>2.0</v>
       </c>
       <c r="I19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20">
@@ -951,7 +946,7 @@
         <v>0</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C20" t="n">
         <v>0.0</v>
@@ -970,22 +965,22 @@
         <v>2.0</v>
       </c>
       <c r="I20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21">
@@ -993,7 +988,7 @@
         <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" t="n">
         <v>0.0</v>
@@ -1012,22 +1007,22 @@
         <v>2.0</v>
       </c>
       <c r="I21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22">
@@ -1035,7 +1030,7 @@
         <v>0</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C22" t="n">
         <v>0.0</v>
@@ -1054,22 +1049,22 @@
         <v>2.0</v>
       </c>
       <c r="I22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23">
@@ -1077,7 +1072,7 @@
         <v>0</v>
       </c>
       <c r="B23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C23" t="n">
         <v>0.0</v>
@@ -1096,22 +1091,22 @@
         <v>2.0</v>
       </c>
       <c r="I23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Un peu de travaille sur le bug classement
</commit_message>
<xml_diff>
--- a/Classeur1.xlsx
+++ b/Classeur1.xlsx
@@ -17,7 +17,7 @@
     <t>4444</t>
   </si>
   <si>
-    <t>bernat</t>
+    <t>xernat</t>
   </si>
   <si>
     <t>rocher</t>
@@ -137,79 +137,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:N23"/>
+  <dimension ref="A2:N24"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1"/>
-      <c r="F1" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="G1" t="n">
-        <v>15.0</v>
-      </c>
-      <c r="H1" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="I1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L1" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" t="s">
-        <v>4</v>
-      </c>
-      <c r="N1" t="s">
-        <v>4</v>
-      </c>
-    </row>
     <row r="2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
         <v>0.0</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E2"/>
       <c r="F2" t="n">
         <v>0.0</v>
       </c>
       <c r="G2" t="n">
-        <v>32.0</v>
+        <v>26.0</v>
       </c>
       <c r="H2" t="n">
-        <v>4.0</v>
+        <v>8.0</v>
       </c>
       <c r="I2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J2" t="s">
         <v>3</v>
@@ -224,7 +182,7 @@
         <v>4</v>
       </c>
       <c r="N2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
@@ -232,41 +190,41 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C3" t="n">
         <v>0.0</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E3"/>
       <c r="F3" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="G3" t="n">
-        <v>5.0</v>
+        <v>32.0</v>
       </c>
       <c r="H3" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="I3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" t="s">
         <v>3</v>
       </c>
-      <c r="J3" t="s">
-        <v>4</v>
-      </c>
       <c r="K3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M3" t="s">
         <v>4</v>
       </c>
       <c r="N3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
@@ -274,7 +232,7 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" t="n">
         <v>0.0</v>
@@ -287,13 +245,13 @@
         <v>1.0</v>
       </c>
       <c r="G4" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="H4" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="I4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J4" t="s">
         <v>4</v>
@@ -316,7 +274,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" t="n">
         <v>0.0</v>
@@ -358,7 +316,7 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" t="n">
         <v>0.0</v>
@@ -400,7 +358,7 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" t="n">
         <v>0.0</v>
@@ -442,7 +400,7 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" t="n">
         <v>0.0</v>
@@ -484,7 +442,7 @@
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" t="n">
         <v>0.0</v>
@@ -526,7 +484,7 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" t="n">
         <v>0.0</v>
@@ -539,7 +497,7 @@
         <v>1.0</v>
       </c>
       <c r="G10" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="H10" t="n">
         <v>2.0</v>
@@ -568,7 +526,7 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" t="n">
         <v>0.0</v>
@@ -584,10 +542,10 @@
         <v>5.0</v>
       </c>
       <c r="H11" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="I11" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J11" t="s">
         <v>4</v>
@@ -652,7 +610,7 @@
         <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" t="n">
         <v>0.0</v>
@@ -665,13 +623,13 @@
         <v>1.0</v>
       </c>
       <c r="G13" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="H13" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="I13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J13" t="s">
         <v>4</v>
@@ -694,7 +652,7 @@
         <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" t="n">
         <v>0.0</v>
@@ -736,7 +694,7 @@
         <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" t="n">
         <v>0.0</v>
@@ -778,7 +736,7 @@
         <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" t="n">
         <v>0.0</v>
@@ -791,7 +749,7 @@
         <v>1.0</v>
       </c>
       <c r="G16" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="H16" t="n">
         <v>2.0</v>
@@ -820,7 +778,7 @@
         <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" t="n">
         <v>0.0</v>
@@ -833,7 +791,7 @@
         <v>1.0</v>
       </c>
       <c r="G17" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="H17" t="n">
         <v>2.0</v>
@@ -862,7 +820,7 @@
         <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" t="n">
         <v>0.0</v>
@@ -904,7 +862,7 @@
         <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C19" t="n">
         <v>0.0</v>
@@ -946,7 +904,7 @@
         <v>0</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20" t="n">
         <v>0.0</v>
@@ -988,7 +946,7 @@
         <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C21" t="n">
         <v>0.0</v>
@@ -1001,7 +959,7 @@
         <v>1.0</v>
       </c>
       <c r="G21" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="H21" t="n">
         <v>2.0</v>
@@ -1030,7 +988,7 @@
         <v>0</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C22" t="n">
         <v>0.0</v>
@@ -1043,7 +1001,7 @@
         <v>1.0</v>
       </c>
       <c r="G22" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="H22" t="n">
         <v>2.0</v>
@@ -1072,7 +1030,7 @@
         <v>0</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C23" t="n">
         <v>0.0</v>
@@ -1085,27 +1043,69 @@
         <v>1.0</v>
       </c>
       <c r="G23" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H23" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="I23" t="s">
+        <v>4</v>
+      </c>
+      <c r="J23" t="s">
+        <v>4</v>
+      </c>
+      <c r="K23" t="s">
+        <v>4</v>
+      </c>
+      <c r="L23" t="s">
+        <v>4</v>
+      </c>
+      <c r="M23" t="s">
+        <v>4</v>
+      </c>
+      <c r="N23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24"/>
+      <c r="F24" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G24" t="n">
         <v>5.0</v>
       </c>
-      <c r="H23" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="I23" t="s">
-        <v>4</v>
-      </c>
-      <c r="J23" t="s">
-        <v>4</v>
-      </c>
-      <c r="K23" t="s">
-        <v>4</v>
-      </c>
-      <c r="L23" t="s">
-        <v>4</v>
-      </c>
-      <c r="M23" t="s">
-        <v>4</v>
-      </c>
-      <c r="N23" t="s">
+      <c r="H24" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="I24" t="s">
+        <v>4</v>
+      </c>
+      <c r="J24" t="s">
+        <v>4</v>
+      </c>
+      <c r="K24" t="s">
+        <v>4</v>
+      </c>
+      <c r="L24" t="s">
+        <v>4</v>
+      </c>
+      <c r="M24" t="s">
+        <v>4</v>
+      </c>
+      <c r="N24" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>